<commit_message>
🚀 Mise à jour de la carte avec icônes et couches corrigées
</commit_message>
<xml_diff>
--- a/final_subsector_data.xlsx
+++ b/final_subsector_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Outil de pilotage\Carte\Données\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\carte_vernier_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F57058-494C-4FD2-8647-62EF41076A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93029139-213D-4F5C-B409-5C9F0F56D966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62BF9D98-97AA-4ABE-A57C-8352E96868AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{62BF9D98-97AA-4ABE-A57C-8352E96868AC}"/>
   </bookViews>
   <sheets>
     <sheet name="final_subsector_data" sheetId="1" r:id="rId1"/>
@@ -980,16 +980,16 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="40.54296875" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>6.0893347520000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>6.0788106959999997</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>6.1088704659999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>6.102292769</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>6.1046595899999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>6.1132170080000003</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>6.1020750469999996</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>6.1074419830000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>6.0900689129999996</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>6.0918793640000004</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>6.0986367440000002</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>6.0766310380000004</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>6.0757178070000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>6.0947540849999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>6.0962069559999996</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>6.0910379370000003</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>6.084569353</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>6.0784902120000002</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>6.1046269940000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>6.1107353980000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>6.1132735379999996</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>6.1141231779999998</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>6.0974524790000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>6.1085562629999997</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>

</xml_diff>